<commit_message>
Replaced with a newer version of this file, because Claire spotted a mistake in the previous version.
</commit_message>
<xml_diff>
--- a/orig_data/HenleyLake_YSI_SondeDailyMeans.xlsx
+++ b/orig_data/HenleyLake_YSI_SondeDailyMeans.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10512"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10609"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ClaireCartozzo/Desktop/ILS Research/Directed Research/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/LaCie/2019 Dissertation Data/2019_05_16_HenleyLakeDissertation/Henley Lake Dissertation Graphs and Analysis/HenleyLakePMSI_ModelFiles/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{4CC954C7-DF9A-9D4E-8B6F-6839F28F8CB2}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E75DF2E1-FFAC-DD49-BDBC-994925C0C777}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="480" yWindow="960" windowWidth="25040" windowHeight="14500" xr2:uid="{1560F87D-A2C2-E24C-BBDE-1E0E96235906}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
   <si>
     <t>Collection</t>
   </si>
@@ -103,16 +103,13 @@
   </si>
   <si>
     <t xml:space="preserve">Collection 18 </t>
-  </si>
-  <si>
-    <t>Collection 19</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="2">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -471,12 +468,15 @@
   <dimension ref="A1:L16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:L16"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <cols>
+    <col min="1" max="1" width="12.1640625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -514,7 +514,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:12">
       <c r="A2" s="2" t="s">
         <v>12</v>
       </c>
@@ -552,7 +552,7 @@
         <v>11.483561197916666</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:12">
       <c r="A3" s="2" t="s">
         <v>13</v>
       </c>
@@ -590,7 +590,7 @@
         <v>13.933823529411764</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:12">
       <c r="A4" s="2" t="s">
         <v>14</v>
       </c>
@@ -628,7 +628,7 @@
         <v>12.171223958333334</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:12">
       <c r="A5" s="2" t="s">
         <v>15</v>
       </c>
@@ -666,7 +666,7 @@
         <v>11.868489583333334</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:12">
       <c r="A6" s="2" t="s">
         <v>16</v>
       </c>
@@ -704,7 +704,7 @@
         <v>11.705729166666666</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:12">
       <c r="A7" s="2" t="s">
         <v>17</v>
       </c>
@@ -742,7 +742,7 @@
         <v>11.572265625</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:12">
       <c r="A8" s="2" t="s">
         <v>18</v>
       </c>
@@ -780,7 +780,7 @@
         <v>11.516927083333334</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:12">
       <c r="A9" s="2" t="s">
         <v>19</v>
       </c>
@@ -818,7 +818,7 @@
         <v>11.402994791666666</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:12">
       <c r="A10" s="2" t="s">
         <v>20</v>
       </c>
@@ -856,7 +856,7 @@
         <v>11.246744791666666</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:12">
       <c r="A11" s="2" t="s">
         <v>21</v>
       </c>
@@ -894,195 +894,160 @@
         <v>11.044921875</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:12">
       <c r="A12" s="2" t="s">
         <v>22</v>
       </c>
       <c r="B12" s="3">
-        <v>43082</v>
+        <v>43113</v>
       </c>
       <c r="C12" s="2">
-        <v>4.9724960327148438</v>
+        <v>2.7422714233398438</v>
       </c>
       <c r="D12" s="2">
-        <v>77.310831069946289</v>
+        <v>75.264133056004837</v>
       </c>
       <c r="E12" s="2">
-        <v>3.5801188088953495E-2</v>
+        <v>3.4706171602010727E-2</v>
       </c>
       <c r="F12" s="2">
-        <v>1.7261505126953125E-2</v>
+        <v>0.61801274617513025</v>
       </c>
       <c r="G12" s="2">
-        <v>2.2222172907883455E-3</v>
+        <v>8.5181589083125189E-2</v>
       </c>
       <c r="H12" s="2">
-        <v>4.688995361328125</v>
+        <v>4.8520559469858808</v>
       </c>
       <c r="I12" s="2">
-        <v>7.8053499857584638</v>
+        <v>5.7018483479817705</v>
       </c>
       <c r="J12" s="2">
-        <v>-76.4312744140625</v>
+        <v>-34.20257568359375</v>
       </c>
       <c r="K12" s="2">
-        <v>187.1337890625</v>
+        <v>267.44842529296875</v>
       </c>
       <c r="L12" s="2">
-        <v>10.80078125</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
+        <v>10.615234375</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12">
       <c r="A13" s="2" t="s">
         <v>23</v>
       </c>
       <c r="B13" s="3">
-        <v>43113</v>
+        <v>43168</v>
       </c>
       <c r="C13" s="2">
-        <v>2.7422714233398438</v>
+        <v>4.9917984008789062</v>
       </c>
       <c r="D13" s="2">
-        <v>75.264133056004837</v>
+        <v>75.852214495340988</v>
       </c>
       <c r="E13" s="2">
-        <v>3.4706171602010727E-2</v>
+        <v>3.5097785914937653E-2</v>
       </c>
       <c r="F13" s="2">
-        <v>0.61801274617513025</v>
+        <v>0.64913431803385413</v>
       </c>
       <c r="G13" s="2">
-        <v>8.5181589083125189E-2</v>
+        <v>8.2874354052667812E-2</v>
       </c>
       <c r="H13" s="2">
-        <v>4.8520559469858808</v>
+        <v>4.990926106770833</v>
       </c>
       <c r="I13" s="2">
-        <v>5.7018483479817705</v>
+        <v>6.0001996358235674</v>
       </c>
       <c r="J13" s="2">
-        <v>-34.20257568359375</v>
+        <v>-40.006001790364586</v>
       </c>
       <c r="K13" s="2">
-        <v>267.44842529296875</v>
+        <v>213.24666341145834</v>
       </c>
       <c r="L13" s="2">
-        <v>10.615234375</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
+        <v>10.358072916666666</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12">
       <c r="A14" s="2" t="s">
         <v>24</v>
       </c>
       <c r="B14" s="3">
-        <v>43168</v>
+        <v>43211</v>
       </c>
       <c r="C14" s="2">
-        <v>4.9917984008789062</v>
+        <v>6.9557571411132812</v>
       </c>
       <c r="D14" s="2">
-        <v>75.852214495340988</v>
+        <v>77.585502306620285</v>
       </c>
       <c r="E14" s="2">
-        <v>3.5097785914937653E-2</v>
+        <v>3.5988683346658945E-2</v>
       </c>
       <c r="F14" s="2">
-        <v>0.64913431803385413</v>
+        <v>1.2404441833496094</v>
       </c>
       <c r="G14" s="2">
-        <v>8.2874354052667812E-2</v>
+        <v>0.15074666899939379</v>
       </c>
       <c r="H14" s="2">
-        <v>4.990926106770833</v>
+        <v>5.0037282307942705</v>
       </c>
       <c r="I14" s="2">
-        <v>6.0001996358235674</v>
+        <v>5.8797162373860674</v>
       </c>
       <c r="J14" s="2">
-        <v>-40.006001790364586</v>
+        <v>-37.419637044270836</v>
       </c>
       <c r="K14" s="2">
-        <v>213.24666341145834</v>
+        <v>370.41219075520831</v>
       </c>
       <c r="L14" s="2">
-        <v>10.358072916666666</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
+        <v>10.05859375</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12">
       <c r="A15" s="2" t="s">
         <v>25</v>
       </c>
       <c r="B15" s="3">
-        <v>43211</v>
+        <v>43247</v>
       </c>
       <c r="C15" s="2">
-        <v>6.9557571411132812</v>
+        <v>8.8184738159179688</v>
       </c>
       <c r="D15" s="2">
-        <v>77.585502306620285</v>
+        <v>89.033030192057296</v>
       </c>
       <c r="E15" s="2">
-        <v>3.5988683346658945E-2</v>
+        <v>4.1544690262526274E-2</v>
       </c>
       <c r="F15" s="2">
-        <v>1.2404441833496094</v>
+        <v>3.032557169596354</v>
       </c>
       <c r="G15" s="2">
-        <v>0.15074666899939379</v>
+        <v>0.35214514657855034</v>
       </c>
       <c r="H15" s="2">
-        <v>5.0037282307942705</v>
+        <v>5.1285654703776045</v>
       </c>
       <c r="I15" s="2">
-        <v>5.8797162373860674</v>
+        <v>5.1006863911946612</v>
       </c>
       <c r="J15" s="2">
-        <v>-37.419637044270836</v>
+        <v>-21.341959635416668</v>
       </c>
       <c r="K15" s="2">
-        <v>370.41219075520831</v>
+        <v>579.98402913411462</v>
       </c>
       <c r="L15" s="2">
-        <v>10.05859375</v>
-      </c>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A16" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="B16" s="3">
-        <v>43247</v>
-      </c>
-      <c r="C16" s="2">
-        <v>8.8184738159179688</v>
-      </c>
-      <c r="D16" s="2">
-        <v>89.033030192057296</v>
-      </c>
-      <c r="E16" s="2">
-        <v>4.1544690262526274E-2</v>
-      </c>
-      <c r="F16" s="2">
-        <v>3.032557169596354</v>
-      </c>
-      <c r="G16" s="2">
-        <v>0.35214514657855034</v>
-      </c>
-      <c r="H16" s="2">
-        <v>5.1285654703776045</v>
-      </c>
-      <c r="I16" s="2">
-        <v>5.1006863911946612</v>
-      </c>
-      <c r="J16" s="2">
-        <v>-21.341959635416668</v>
-      </c>
-      <c r="K16" s="2">
-        <v>579.98402913411462</v>
-      </c>
-      <c r="L16" s="2">
         <v>9.765625</v>
       </c>
+    </row>
+    <row r="16" spans="1:12">
+      <c r="A16" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>